<commit_message>
Se registraron las no conformidades de la auditoria de requerimientos
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/inter_Cabina/5. Aseguramiento de la Calidad/Inter_cabina_Auditoria_150604.xlsx
+++ b/Proyectos/Activos/inter_Cabina/5. Aseguramiento de la Calidad/Inter_cabina_Auditoria_150604.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="144" windowWidth="15876" windowHeight="5328"/>
+    <workbookView xWindow="288" yWindow="144" windowWidth="15876" windowHeight="5328" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Inf. Gral." sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="180">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t>No se han realizado líneas base</t>
+  </si>
+  <si>
+    <t>No se tiene el manual de requerimientos firmado por el cliente</t>
+  </si>
+  <si>
+    <t>No se tienen los requerimientos firmados por el cliente</t>
   </si>
 </sst>
 </file>
@@ -1129,6 +1135,24 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1144,26 +1168,11 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1172,9 +1181,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1518,7 +1524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1537,76 +1543,76 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="62"/>
     </row>
     <row r="6" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="60">
+      <c r="C7" s="63">
         <v>42159</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="54"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="54"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="29" t="s">
@@ -1705,11 +1711,11 @@
     </row>
     <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
     </row>
     <row r="21" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="28" t="s">
@@ -1808,11 +1814,11 @@
     </row>
     <row r="28" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
       <c r="E29" s="21"/>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
@@ -1877,11 +1883,11 @@
     </row>
     <row r="34" spans="2:5" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="2:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -1920,9 +1926,9 @@
         <f>COUNTA(Funcional!D11:D18)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="33" t="e">
+      <c r="D38" s="33">
         <f>COUNTIF((Funcional!D11:D18),"x")/(COUNTIF((Funcional!D11:D18),"x")+COUNTIF((Funcional!E11:E18),"x"))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -1943,16 +1949,16 @@
     <row r="41" spans="2:5" s="23" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -1993,22 +1999,22 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65" t="s">
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="41" t="s">
         <v>5</v>
       </c>
@@ -2018,17 +2024,17 @@
       <c r="F3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="65"/>
+      <c r="G3" s="66"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
@@ -2128,10 +2134,10 @@
         <v>28</v>
       </c>
       <c r="C12" s="69"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
@@ -2284,10 +2290,10 @@
         <v>60</v>
       </c>
       <c r="C25" s="69"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
@@ -2401,10 +2407,10 @@
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="64"/>
+      <c r="C35" s="65"/>
       <c r="D35" s="42"/>
       <c r="E35" s="42"/>
       <c r="F35" s="42"/>
@@ -2436,14 +2442,14 @@
       <c r="G37" s="13"/>
     </row>
     <row r="39" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="10">
@@ -2540,14 +2546,14 @@
       <c r="C47" s="38"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="64" t="s">
+      <c r="B48" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="10">
@@ -2602,13 +2608,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D39:E39"/>
@@ -2621,6 +2620,13 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <conditionalFormatting sqref="D24:F24 D26:F34">
     <cfRule type="expression" dxfId="2" priority="8" stopIfTrue="1">
@@ -2642,7 +2648,7 @@
   <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2669,22 +2675,22 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="70"/>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65" t="s">
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="70"/>
-      <c r="C3" s="65"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="41" t="s">
         <v>5</v>
       </c>
@@ -2694,18 +2700,18 @@
       <c r="F3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="65"/>
+      <c r="G3" s="66"/>
     </row>
     <row r="4" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
@@ -2852,7 +2858,7 @@
       <c r="F13" s="35"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="10">
         <f t="shared" si="0"/>
@@ -2867,7 +2873,7 @@
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="51" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2881,14 +2887,14 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
@@ -3124,14 +3130,14 @@
     </row>
     <row r="34" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
@@ -3241,14 +3247,14 @@
     </row>
     <row r="43" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="67" t="s">
+      <c r="B43" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="67"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
@@ -3582,14 +3588,14 @@
     </row>
     <row r="68" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
-      <c r="B68" s="67" t="s">
+      <c r="B68" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="67"/>
-      <c r="D68" s="67"/>
-      <c r="E68" s="67"/>
-      <c r="F68" s="67"/>
-      <c r="G68" s="67"/>
+      <c r="C68" s="64"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" s="10">
@@ -3698,14 +3704,14 @@
       <c r="C77" s="18"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="67" t="s">
+      <c r="B78" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C78" s="67"/>
-      <c r="D78" s="67"/>
-      <c r="E78" s="67"/>
-      <c r="F78" s="67"/>
-      <c r="G78" s="67"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="64"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B79" s="10">
@@ -3773,12 +3779,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="B68:C68"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B34:C34"/>
@@ -3795,6 +3795,12 @@
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="F43:G43"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="B68:C68"/>
   </mergeCells>
   <conditionalFormatting sqref="C77">
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
@@ -3810,8 +3816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3831,16 +3837,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65" t="s">
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="4"/>
@@ -3861,7 +3867,7 @@
       <c r="F3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="65"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -3869,21 +3875,21 @@
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="2:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B5" s="44">
         <v>1</v>
       </c>
@@ -3907,7 +3913,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B6" s="44">
         <v>2</v>
       </c>
@@ -3966,14 +3972,14 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
       <c r="H9" s="4"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -4084,14 +4090,14 @@
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="4"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -4129,11 +4135,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="B15:C15"/>
@@ -4141,6 +4142,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -4153,8 +4159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4170,22 +4176,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65" t="s">
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="41" t="s">
         <v>5</v>
       </c>
@@ -4195,17 +4201,17 @@
       <c r="F3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="65"/>
+      <c r="G3" s="66"/>
     </row>
     <row r="4" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
@@ -4280,14 +4286,14 @@
       <c r="G9" s="46"/>
     </row>
     <row r="10" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
@@ -4388,7 +4394,7 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <f>+B17+1</f>
         <v>8</v>
@@ -4397,11 +4403,13 @@
         <v>69</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="G18" s="51"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="51" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="46"/>
@@ -4412,14 +4420,14 @@
       <c r="G19" s="46"/>
     </row>
     <row r="20" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
@@ -4516,12 +4524,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
+    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4609,24 +4623,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
-    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BF54FE-89ED-4BFD-984C-5255D8E3B158}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B74BF6BA-412C-41A7-B0A7-7E1FCDB78793}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4649,16 +4664,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B74BF6BA-412C-41A7-B0A7-7E1FCDB78793}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BF54FE-89ED-4BFD-984C-5255D8E3B158}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>